<commit_message>
Scripting Setup Broker and Setup PIC Broker
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV031-001 - Setup Broker Investasi - General Tambah Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV031-001 - Setup Broker Investasi - General Tambah Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8455BBF8-48B7-4149-93E4-C0C7F172FA81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FBF408-43A1-4B4A-BD83-AECFD5276A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>Tidak</t>
-  </si>
-  <si>
-    <t>008 - Bank Mandiri</t>
   </si>
   <si>
     <t>01</t>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>Analisis Investasi</t>
+  </si>
+  <si>
+    <t>008 : Bank Mandiri</t>
   </si>
 </sst>
 </file>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="T2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +605,7 @@
     <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.7109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
@@ -661,7 +661,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
@@ -724,10 +724,10 @@
         <v>32</v>
       </c>
       <c r="AD1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="409.5" x14ac:dyDescent="0.25">
@@ -735,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -744,19 +744,19 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G2" s="4">
         <v>31246</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>11</v>
@@ -801,28 +801,28 @@
         <v>36</v>
       </c>
       <c r="X2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="AA2" s="1">
         <v>12131313131</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="AD2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>